<commit_message>
Test - no changes
</commit_message>
<xml_diff>
--- a/Behaviour/bcio_behaviour.xlsx
+++ b/Behaviour/bcio_behaviour.xlsx
@@ -621,11 +621,13 @@
       <c r="R2" s="2" t="inlineStr"/>
       <c r="S2" s="2" t="inlineStr"/>
       <c r="T2" s="2" t="inlineStr"/>
-      <c r="U2" s="2" t="inlineStr"/>
+      <c r="U2" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="V2" s="2" t="inlineStr"/>
       <c r="W2" s="2" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>PS; BG</t>
         </is>
       </c>
       <c r="X2" s="2" t="inlineStr">
@@ -681,7 +683,9 @@
       <c r="R3" s="2" t="inlineStr"/>
       <c r="S3" s="2" t="inlineStr"/>
       <c r="T3" s="2" t="inlineStr"/>
-      <c r="U3" s="2" t="inlineStr"/>
+      <c r="U3" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="V3" s="2" t="inlineStr"/>
       <c r="W3" s="2" t="inlineStr">
         <is>
@@ -741,7 +745,9 @@
       <c r="R4" s="2" t="inlineStr"/>
       <c r="S4" s="2" t="inlineStr"/>
       <c r="T4" s="2" t="inlineStr"/>
-      <c r="U4" s="2" t="inlineStr"/>
+      <c r="U4" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="V4" s="2" t="inlineStr"/>
       <c r="W4" s="2" t="inlineStr">
         <is>
@@ -801,7 +807,9 @@
       <c r="R5" s="2" t="inlineStr"/>
       <c r="S5" s="2" t="inlineStr"/>
       <c r="T5" s="2" t="inlineStr"/>
-      <c r="U5" s="2" t="inlineStr"/>
+      <c r="U5" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="V5" s="2" t="inlineStr"/>
       <c r="W5" s="2" t="inlineStr">
         <is>
@@ -1421,7 +1429,9 @@
       <c r="R15" s="2" t="inlineStr"/>
       <c r="S15" s="2" t="inlineStr"/>
       <c r="T15" s="2" t="inlineStr"/>
-      <c r="U15" s="2" t="inlineStr"/>
+      <c r="U15" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="V15" s="2" t="inlineStr"/>
       <c r="W15" s="2" t="inlineStr">
         <is>
@@ -1481,7 +1491,9 @@
       <c r="R16" s="2" t="inlineStr"/>
       <c r="S16" s="2" t="inlineStr"/>
       <c r="T16" s="2" t="inlineStr"/>
-      <c r="U16" s="2" t="inlineStr"/>
+      <c r="U16" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="V16" s="2" t="inlineStr"/>
       <c r="W16" s="2" t="inlineStr">
         <is>
@@ -1689,7 +1701,9 @@
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
+      <c r="U19" t="n">
+        <v>0</v>
+      </c>
       <c r="V19" t="inlineStr"/>
       <c r="W19" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Removed line break in relation name
</commit_message>
<xml_diff>
--- a/Behaviour/bcio_behaviour.xlsx
+++ b/Behaviour/bcio_behaviour.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcjtpms_ucl_ac_uk/Documents/Documents/GitHub/ontologies/Behaviour/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgehrk/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_45F5E5BEDD0A5433ADAE3C33565ED87656C95860" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE2127AE-F81B-4746-B616-C074B5DEF37B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3A95DB-EFE6-B94E-B9BF-D79104D47173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="165" windowWidth="23925" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -2347,8 +2347,7 @@
     <t>REL 'has behavioural attribute'</t>
   </si>
   <si>
-    <t>REL 'has abstinence
-period'</t>
+    <t>REL 'has abstinence period'</t>
   </si>
 </sst>
 </file>
@@ -2400,12 +2399,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2711,12 +2709,12 @@
   <dimension ref="A1:Y180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2756,7 +2754,7 @@
       <c r="M1" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>765</v>
       </c>
       <c r="O1" s="1" t="s">
@@ -2793,7 +2791,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -2839,7 +2837,7 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
@@ -2885,7 +2883,7 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -2932,7 +2930,7 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>45</v>
       </c>
@@ -2978,7 +2976,7 @@
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -3022,7 +3020,7 @@
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
@@ -3066,7 +3064,7 @@
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>60</v>
       </c>
@@ -3108,7 +3106,7 @@
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>64</v>
       </c>
@@ -3150,7 +3148,7 @@
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>70</v>
       </c>
@@ -3196,7 +3194,7 @@
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>76</v>
       </c>
@@ -3240,7 +3238,7 @@
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>81</v>
       </c>
@@ -3282,7 +3280,7 @@
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>85</v>
       </c>
@@ -3324,7 +3322,7 @@
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>89</v>
       </c>
@@ -3366,7 +3364,7 @@
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>93</v>
       </c>
@@ -3412,7 +3410,7 @@
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>97</v>
       </c>
@@ -3458,7 +3456,7 @@
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>101</v>
       </c>
@@ -3506,7 +3504,7 @@
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>108</v>
       </c>
@@ -3556,7 +3554,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>116</v>
       </c>
@@ -3600,7 +3598,7 @@
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>121</v>
       </c>
@@ -3646,7 +3644,7 @@
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>126</v>
       </c>
@@ -3692,7 +3690,7 @@
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>133</v>
       </c>
@@ -3736,7 +3734,7 @@
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>137</v>
       </c>
@@ -3780,7 +3778,7 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>143</v>
       </c>
@@ -3828,7 +3826,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>151</v>
       </c>
@@ -3872,7 +3870,7 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>156</v>
       </c>
@@ -3916,7 +3914,7 @@
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>161</v>
       </c>
@@ -3960,7 +3958,7 @@
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>165</v>
       </c>
@@ -4004,7 +4002,7 @@
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>170</v>
       </c>
@@ -4050,7 +4048,7 @@
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>176</v>
       </c>
@@ -4094,7 +4092,7 @@
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>180</v>
       </c>
@@ -4138,7 +4136,7 @@
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>184</v>
       </c>
@@ -4186,7 +4184,7 @@
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>190</v>
       </c>
@@ -4230,7 +4228,7 @@
       <c r="X33" s="2"/>
       <c r="Y33" s="2"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>194</v>
       </c>
@@ -4274,7 +4272,7 @@
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>198</v>
       </c>
@@ -4318,7 +4316,7 @@
       <c r="X35" s="2"/>
       <c r="Y35" s="2"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>202</v>
       </c>
@@ -4360,7 +4358,7 @@
       <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>205</v>
       </c>
@@ -4404,7 +4402,7 @@
       <c r="X37" s="2"/>
       <c r="Y37" s="2"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>209</v>
       </c>
@@ -4446,7 +4444,7 @@
       <c r="X38" s="2"/>
       <c r="Y38" s="2"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>212</v>
       </c>
@@ -4488,7 +4486,7 @@
       <c r="X39" s="2"/>
       <c r="Y39" s="2"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>216</v>
       </c>
@@ -4532,7 +4530,7 @@
       <c r="X40" s="2"/>
       <c r="Y40" s="2"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>221</v>
       </c>
@@ -4574,7 +4572,7 @@
       <c r="X41" s="2"/>
       <c r="Y41" s="2"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>224</v>
       </c>
@@ -4622,7 +4620,7 @@
       <c r="X42" s="2"/>
       <c r="Y42" s="2"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>230</v>
       </c>
@@ -4664,7 +4662,7 @@
       <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>233</v>
       </c>
@@ -4710,7 +4708,7 @@
       <c r="X44" s="2"/>
       <c r="Y44" s="2"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>238</v>
       </c>
@@ -4756,7 +4754,7 @@
       <c r="X45" s="2"/>
       <c r="Y45" s="2"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>244</v>
       </c>
@@ -4800,7 +4798,7 @@
       <c r="X46" s="2"/>
       <c r="Y46" s="2"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>248</v>
       </c>
@@ -4850,7 +4848,7 @@
       <c r="X47" s="2"/>
       <c r="Y47" s="2"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>254</v>
       </c>
@@ -4894,7 +4892,7 @@
       <c r="X48" s="2"/>
       <c r="Y48" s="2"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>258</v>
       </c>
@@ -4936,7 +4934,7 @@
       <c r="X49" s="2"/>
       <c r="Y49" s="2"/>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>261</v>
       </c>
@@ -4978,7 +4976,7 @@
       <c r="X50" s="2"/>
       <c r="Y50" s="2"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>263</v>
       </c>
@@ -5024,7 +5022,7 @@
       <c r="X51" s="2"/>
       <c r="Y51" s="2"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>268</v>
       </c>
@@ -5053,7 +5051,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>271</v>
       </c>
@@ -5097,7 +5095,7 @@
       <c r="X53" s="2"/>
       <c r="Y53" s="2"/>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>275</v>
       </c>
@@ -5139,7 +5137,7 @@
       <c r="X54" s="2"/>
       <c r="Y54" s="2"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>278</v>
       </c>
@@ -5183,7 +5181,7 @@
       <c r="X55" s="2"/>
       <c r="Y55" s="2"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>283</v>
       </c>
@@ -5227,7 +5225,7 @@
       <c r="X56" s="2"/>
       <c r="Y56" s="2"/>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>287</v>
       </c>
@@ -5273,7 +5271,7 @@
       <c r="X57" s="2"/>
       <c r="Y57" s="2"/>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>292</v>
       </c>
@@ -5315,7 +5313,7 @@
       <c r="X58" s="2"/>
       <c r="Y58" s="2"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>295</v>
       </c>
@@ -5359,7 +5357,7 @@
       <c r="X59" s="2"/>
       <c r="Y59" s="2"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>300</v>
       </c>
@@ -5403,7 +5401,7 @@
       <c r="X60" s="2"/>
       <c r="Y60" s="2"/>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>304</v>
       </c>
@@ -5447,7 +5445,7 @@
       <c r="X61" s="2"/>
       <c r="Y61" s="2"/>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>308</v>
       </c>
@@ -5491,7 +5489,7 @@
       <c r="X62" s="2"/>
       <c r="Y62" s="2"/>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>313</v>
       </c>
@@ -5533,7 +5531,7 @@
       <c r="X63" s="2"/>
       <c r="Y63" s="2"/>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>316</v>
       </c>
@@ -5579,7 +5577,7 @@
       <c r="X64" s="2"/>
       <c r="Y64" s="2"/>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>321</v>
       </c>
@@ -5625,7 +5623,7 @@
       <c r="X65" s="2"/>
       <c r="Y65" s="2"/>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>327</v>
       </c>
@@ -5671,7 +5669,7 @@
       <c r="X66" s="2"/>
       <c r="Y66" s="2"/>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>332</v>
       </c>
@@ -5720,7 +5718,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>338</v>
       </c>
@@ -5772,7 +5770,7 @@
       <c r="X68" s="2"/>
       <c r="Y68" s="2"/>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>346</v>
       </c>
@@ -5824,7 +5822,7 @@
       <c r="X69" s="2"/>
       <c r="Y69" s="2"/>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>354</v>
       </c>
@@ -5874,7 +5872,7 @@
       <c r="X70" s="2"/>
       <c r="Y70" s="2"/>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>360</v>
       </c>
@@ -5916,7 +5914,7 @@
       <c r="X71" s="2"/>
       <c r="Y71" s="2"/>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>363</v>
       </c>
@@ -5962,7 +5960,7 @@
       <c r="X72" s="2"/>
       <c r="Y72" s="2"/>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>368</v>
       </c>
@@ -6006,7 +6004,7 @@
       <c r="X73" s="2"/>
       <c r="Y73" s="2"/>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>371</v>
       </c>
@@ -6048,7 +6046,7 @@
       <c r="X74" s="2"/>
       <c r="Y74" s="2"/>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>375</v>
       </c>
@@ -6092,7 +6090,7 @@
       <c r="X75" s="2"/>
       <c r="Y75" s="2"/>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>380</v>
       </c>
@@ -6136,7 +6134,7 @@
       <c r="X76" s="2"/>
       <c r="Y76" s="2"/>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>384</v>
       </c>
@@ -6182,7 +6180,7 @@
       <c r="X77" s="2"/>
       <c r="Y77" s="2"/>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>387</v>
       </c>
@@ -6224,7 +6222,7 @@
       <c r="X78" s="2"/>
       <c r="Y78" s="2"/>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>389</v>
       </c>
@@ -6266,7 +6264,7 @@
       <c r="X79" s="2"/>
       <c r="Y79" s="2"/>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>392</v>
       </c>
@@ -6312,7 +6310,7 @@
       <c r="X80" s="2"/>
       <c r="Y80" s="2"/>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>397</v>
       </c>
@@ -6356,7 +6354,7 @@
       <c r="X81" s="2"/>
       <c r="Y81" s="2"/>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>401</v>
       </c>
@@ -6400,7 +6398,7 @@
       <c r="X82" s="2"/>
       <c r="Y82" s="2"/>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>405</v>
       </c>
@@ -6444,7 +6442,7 @@
       <c r="X83" s="2"/>
       <c r="Y83" s="2"/>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>409</v>
       </c>
@@ -6488,7 +6486,7 @@
       <c r="X84" s="2"/>
       <c r="Y84" s="2"/>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>413</v>
       </c>
@@ -6530,7 +6528,7 @@
       <c r="X85" s="2"/>
       <c r="Y85" s="2"/>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>418</v>
       </c>
@@ -6572,7 +6570,7 @@
       <c r="X86" s="2"/>
       <c r="Y86" s="2"/>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>421</v>
       </c>
@@ -6616,7 +6614,7 @@
       <c r="X87" s="2"/>
       <c r="Y87" s="2"/>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>425</v>
       </c>
@@ -6658,7 +6656,7 @@
       <c r="X88" s="2"/>
       <c r="Y88" s="2"/>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>427</v>
       </c>
@@ -6704,7 +6702,7 @@
       <c r="X89" s="2"/>
       <c r="Y89" s="2"/>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>432</v>
       </c>
@@ -6750,7 +6748,7 @@
       <c r="X90" s="2"/>
       <c r="Y90" s="2"/>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>436</v>
       </c>
@@ -6794,7 +6792,7 @@
       <c r="X91" s="2"/>
       <c r="Y91" s="2"/>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>440</v>
       </c>
@@ -6838,7 +6836,7 @@
       <c r="X92" s="2"/>
       <c r="Y92" s="2"/>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>444</v>
       </c>
@@ -6882,7 +6880,7 @@
       <c r="X93" s="2"/>
       <c r="Y93" s="2"/>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>448</v>
       </c>
@@ -6926,7 +6924,7 @@
       <c r="X94" s="2"/>
       <c r="Y94" s="2"/>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>452</v>
       </c>
@@ -6970,7 +6968,7 @@
       <c r="X95" s="2"/>
       <c r="Y95" s="2"/>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>456</v>
       </c>
@@ -7012,7 +7010,7 @@
       <c r="X96" s="2"/>
       <c r="Y96" s="2"/>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>459</v>
       </c>
@@ -7054,7 +7052,7 @@
       <c r="X97" s="2"/>
       <c r="Y97" s="2"/>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>462</v>
       </c>
@@ -7096,7 +7094,7 @@
       <c r="X98" s="2"/>
       <c r="Y98" s="2"/>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>466</v>
       </c>
@@ -7138,7 +7136,7 @@
       <c r="X99" s="2"/>
       <c r="Y99" s="2"/>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>469</v>
       </c>
@@ -7184,7 +7182,7 @@
       <c r="X100" s="2"/>
       <c r="Y100" s="2"/>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>476</v>
       </c>
@@ -7226,7 +7224,7 @@
       <c r="X101" s="2"/>
       <c r="Y101" s="2"/>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>479</v>
       </c>
@@ -7272,7 +7270,7 @@
       <c r="X102" s="2"/>
       <c r="Y102" s="2"/>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>484</v>
       </c>
@@ -7318,7 +7316,7 @@
       <c r="X103" s="2"/>
       <c r="Y103" s="2"/>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>489</v>
       </c>
@@ -7364,7 +7362,7 @@
       <c r="X104" s="2"/>
       <c r="Y104" s="2"/>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>494</v>
       </c>
@@ -7412,7 +7410,7 @@
       <c r="X105" s="2"/>
       <c r="Y105" s="2"/>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>499</v>
       </c>
@@ -7454,7 +7452,7 @@
       <c r="X106" s="2"/>
       <c r="Y106" s="2"/>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>501</v>
       </c>
@@ -7496,7 +7494,7 @@
       <c r="X107" s="2"/>
       <c r="Y107" s="2"/>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>505</v>
       </c>
@@ -7540,7 +7538,7 @@
       <c r="X108" s="2"/>
       <c r="Y108" s="2"/>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>510</v>
       </c>
@@ -7586,7 +7584,7 @@
       <c r="X109" s="2"/>
       <c r="Y109" s="2"/>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>514</v>
       </c>
@@ -7630,7 +7628,7 @@
       <c r="X110" s="2"/>
       <c r="Y110" s="2"/>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>518</v>
       </c>
@@ -7672,7 +7670,7 @@
       <c r="X111" s="2"/>
       <c r="Y111" s="2"/>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>521</v>
       </c>
@@ -7714,7 +7712,7 @@
       <c r="X112" s="2"/>
       <c r="Y112" s="2"/>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>524</v>
       </c>
@@ -7756,7 +7754,7 @@
       <c r="X113" s="2"/>
       <c r="Y113" s="2"/>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>526</v>
       </c>
@@ -7798,7 +7796,7 @@
       <c r="X114" s="2"/>
       <c r="Y114" s="2"/>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>529</v>
       </c>
@@ -7842,7 +7840,7 @@
       <c r="X115" s="2"/>
       <c r="Y115" s="2"/>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>535</v>
       </c>
@@ -7890,7 +7888,7 @@
       <c r="X116" s="2"/>
       <c r="Y116" s="2"/>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>539</v>
       </c>
@@ -7936,7 +7934,7 @@
       <c r="X117" s="2"/>
       <c r="Y117" s="2"/>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>544</v>
       </c>
@@ -7980,7 +7978,7 @@
       <c r="X118" s="2"/>
       <c r="Y118" s="2"/>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>548</v>
       </c>
@@ -8026,7 +8024,7 @@
       <c r="X119" s="2"/>
       <c r="Y119" s="2"/>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>552</v>
       </c>
@@ -8074,7 +8072,7 @@
       <c r="X120" s="2"/>
       <c r="Y120" s="2"/>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>557</v>
       </c>
@@ -8118,7 +8116,7 @@
       <c r="X121" s="2"/>
       <c r="Y121" s="2"/>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>561</v>
       </c>
@@ -8164,7 +8162,7 @@
       <c r="X122" s="2"/>
       <c r="Y122" s="2"/>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>565</v>
       </c>
@@ -8206,7 +8204,7 @@
       <c r="X123" s="2"/>
       <c r="Y123" s="2"/>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>569</v>
       </c>
@@ -8248,7 +8246,7 @@
       <c r="X124" s="2"/>
       <c r="Y124" s="2"/>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>572</v>
       </c>
@@ -8290,7 +8288,7 @@
       <c r="X125" s="2"/>
       <c r="Y125" s="2"/>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>574</v>
       </c>
@@ -8336,7 +8334,7 @@
       <c r="X126" s="2"/>
       <c r="Y126" s="2"/>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>580</v>
       </c>
@@ -8380,7 +8378,7 @@
       <c r="X127" s="2"/>
       <c r="Y127" s="2"/>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>582</v>
       </c>
@@ -8422,7 +8420,7 @@
       <c r="X128" s="2"/>
       <c r="Y128" s="2"/>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>585</v>
       </c>
@@ -8464,7 +8462,7 @@
       <c r="X129" s="2"/>
       <c r="Y129" s="2"/>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>588</v>
       </c>
@@ -8508,7 +8506,7 @@
       <c r="X130" s="2"/>
       <c r="Y130" s="2"/>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>592</v>
       </c>
@@ -8554,7 +8552,7 @@
       <c r="X131" s="2"/>
       <c r="Y131" s="2"/>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>596</v>
       </c>
@@ -8602,7 +8600,7 @@
       <c r="X132" s="2"/>
       <c r="Y132" s="2"/>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>600</v>
       </c>
@@ -8644,7 +8642,7 @@
       <c r="X133" s="2"/>
       <c r="Y133" s="2"/>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>604</v>
       </c>
@@ -8686,7 +8684,7 @@
       <c r="X134" s="2"/>
       <c r="Y134" s="2"/>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>608</v>
       </c>
@@ -8728,7 +8726,7 @@
       <c r="X135" s="2"/>
       <c r="Y135" s="2"/>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>610</v>
       </c>
@@ -8770,7 +8768,7 @@
       <c r="X136" s="2"/>
       <c r="Y136" s="2"/>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>613</v>
       </c>
@@ -8812,7 +8810,7 @@
       <c r="X137" s="2"/>
       <c r="Y137" s="2"/>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>615</v>
       </c>
@@ -8854,7 +8852,7 @@
       <c r="X138" s="2"/>
       <c r="Y138" s="2"/>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>618</v>
       </c>
@@ -8896,7 +8894,7 @@
       <c r="X139" s="2"/>
       <c r="Y139" s="2"/>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>621</v>
       </c>
@@ -8938,7 +8936,7 @@
       <c r="X140" s="2"/>
       <c r="Y140" s="2"/>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>624</v>
       </c>
@@ -8980,7 +8978,7 @@
       <c r="X141" s="2"/>
       <c r="Y141" s="2"/>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>626</v>
       </c>
@@ -9022,7 +9020,7 @@
       <c r="X142" s="2"/>
       <c r="Y142" s="2"/>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>629</v>
       </c>
@@ -9064,7 +9062,7 @@
       <c r="X143" s="2"/>
       <c r="Y143" s="2"/>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>632</v>
       </c>
@@ -9106,7 +9104,7 @@
       <c r="X144" s="2"/>
       <c r="Y144" s="2"/>
     </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>635</v>
       </c>
@@ -9152,7 +9150,7 @@
       <c r="X145" s="2"/>
       <c r="Y145" s="2"/>
     </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>640</v>
       </c>
@@ -9198,7 +9196,7 @@
       <c r="X146" s="2"/>
       <c r="Y146" s="2"/>
     </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>645</v>
       </c>
@@ -9240,7 +9238,7 @@
       <c r="X147" s="2"/>
       <c r="Y147" s="2"/>
     </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>648</v>
       </c>
@@ -9284,7 +9282,7 @@
       <c r="X148" s="2"/>
       <c r="Y148" s="2"/>
     </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>651</v>
       </c>
@@ -9330,7 +9328,7 @@
       <c r="X149" s="2"/>
       <c r="Y149" s="2"/>
     </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>656</v>
       </c>
@@ -9372,7 +9370,7 @@
       <c r="X150" s="2"/>
       <c r="Y150" s="2"/>
     </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>659</v>
       </c>
@@ -9420,7 +9418,7 @@
       <c r="X151" s="2"/>
       <c r="Y151" s="2"/>
     </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>663</v>
       </c>
@@ -9462,7 +9460,7 @@
       <c r="X152" s="2"/>
       <c r="Y152" s="2"/>
     </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>666</v>
       </c>
@@ -9506,7 +9504,7 @@
       <c r="X153" s="2"/>
       <c r="Y153" s="2"/>
     </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>670</v>
       </c>
@@ -9548,7 +9546,7 @@
       <c r="X154" s="2"/>
       <c r="Y154" s="2"/>
     </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>673</v>
       </c>
@@ -9596,7 +9594,7 @@
       <c r="X155" s="2"/>
       <c r="Y155" s="2"/>
     </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>677</v>
       </c>
@@ -9638,7 +9636,7 @@
       <c r="X156" s="2"/>
       <c r="Y156" s="2"/>
     </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>680</v>
       </c>
@@ -9680,7 +9678,7 @@
       <c r="X157" s="2"/>
       <c r="Y157" s="2"/>
     </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>682</v>
       </c>
@@ -9722,7 +9720,7 @@
       <c r="X158" s="2"/>
       <c r="Y158" s="2"/>
     </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>684</v>
       </c>
@@ -9766,7 +9764,7 @@
       <c r="X159" s="2"/>
       <c r="Y159" s="2"/>
     </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>689</v>
       </c>
@@ -9808,7 +9806,7 @@
       <c r="X160" s="2"/>
       <c r="Y160" s="2"/>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>692</v>
       </c>
@@ -9856,7 +9854,7 @@
       <c r="X161" s="2"/>
       <c r="Y161" s="2"/>
     </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>697</v>
       </c>
@@ -9898,7 +9896,7 @@
       <c r="X162" s="2"/>
       <c r="Y162" s="2"/>
     </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>700</v>
       </c>
@@ -9942,7 +9940,7 @@
       <c r="X163" s="2"/>
       <c r="Y163" s="2"/>
     </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>704</v>
       </c>
@@ -9986,7 +9984,7 @@
       <c r="X164" s="2"/>
       <c r="Y164" s="2"/>
     </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>709</v>
       </c>
@@ -10032,7 +10030,7 @@
       <c r="X165" s="2"/>
       <c r="Y165" s="2"/>
     </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>713</v>
       </c>
@@ -10076,7 +10074,7 @@
       <c r="X166" s="2"/>
       <c r="Y166" s="2"/>
     </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>716</v>
       </c>
@@ -10120,7 +10118,7 @@
       <c r="X167" s="2"/>
       <c r="Y167" s="2"/>
     </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>719</v>
       </c>
@@ -10166,7 +10164,7 @@
       <c r="X168" s="2"/>
       <c r="Y168" s="2"/>
     </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>722</v>
       </c>
@@ -10212,7 +10210,7 @@
       <c r="X169" s="2"/>
       <c r="Y169" s="2"/>
     </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>724</v>
       </c>
@@ -10260,7 +10258,7 @@
       <c r="X170" s="2"/>
       <c r="Y170" s="2"/>
     </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>728</v>
       </c>
@@ -10304,7 +10302,7 @@
       <c r="X171" s="2"/>
       <c r="Y171" s="2"/>
     </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>732</v>
       </c>
@@ -10346,7 +10344,7 @@
       <c r="X172" s="2"/>
       <c r="Y172" s="2"/>
     </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>737</v>
       </c>
@@ -10390,7 +10388,7 @@
       <c r="X173" s="2"/>
       <c r="Y173" s="2"/>
     </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>742</v>
       </c>
@@ -10434,7 +10432,7 @@
       <c r="X174" s="2"/>
       <c r="Y174" s="2"/>
     </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>746</v>
       </c>
@@ -10482,7 +10480,7 @@
       <c r="X175" s="2"/>
       <c r="Y175" s="2"/>
     </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>750</v>
       </c>
@@ -10526,7 +10524,7 @@
       <c r="X176" s="2"/>
       <c r="Y176" s="2"/>
     </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>753</v>
       </c>
@@ -10568,7 +10566,7 @@
       <c r="X177" s="2"/>
       <c r="Y177" s="2"/>
     </row>
-    <row r="178" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>755</v>
       </c>
@@ -10610,7 +10608,7 @@
       <c r="X178" s="2"/>
       <c r="Y178" s="2"/>
     </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>757</v>
       </c>
@@ -10654,7 +10652,7 @@
       <c r="X179" s="2"/>
       <c r="Y179" s="2"/>
     </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>760</v>
       </c>

</xml_diff>